<commit_message>
move capture to folder Images
</commit_message>
<xml_diff>
--- a/Plan-Project-CI-CD-Worksheet.xlsx
+++ b/Plan-Project-CI-CD-Worksheet.xlsx
@@ -19,59 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Week</t>
   </si>
   <si>
-    <t>Create a spreadsheet to store my work plan</t>
-  </si>
-  <si>
-    <t>Create a new Trello board for "Building a CI/CD Pipeline" project</t>
-  </si>
-  <si>
-    <t>Create a new repo: "Building a CI/CD Pipeline" to store my code</t>
-  </si>
-  <si>
-    <t>Create the Makefile for my "Building a CI/CD Pipeline" repo</t>
-  </si>
-  <si>
-    <t>Create the requirements.txt file for my repo</t>
-  </si>
-  <si>
-    <t>Create hello.py and test_hello.py file for my repo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task work </t>
-  </si>
-  <si>
-    <t>Download and push Flask code to my repo</t>
-  </si>
-  <si>
-    <t>Set up GitHub Actions: create main.yml for run after push code and take run successful screenshot</t>
-  </si>
-  <si>
-    <t>Add the GitHub Actions badge to the README file in my repo</t>
-  </si>
-  <si>
-    <t>Update make_predict_azure_app.sh</t>
-  </si>
-  <si>
-    <t>Setting environment and run app</t>
-  </si>
-  <si>
-    <t>Push app to App Service in Azure</t>
-  </si>
-  <si>
-    <t>Goals</t>
-  </si>
-  <si>
-    <t>Finish my project 2 DevOps</t>
-  </si>
-  <si>
-    <t>Set up the Azure DevOps pipeline and makesure it working</t>
-  </si>
-  <si>
     <t>17/11/2022</t>
   </si>
   <si>
@@ -81,20 +33,90 @@
     <t>28/11/2022</t>
   </si>
   <si>
-    <t>Update document with README file</t>
-  </si>
-  <si>
-    <t>Submit  project 2 DevOps</t>
-  </si>
-  <si>
-    <t>Create the Python Virtual Environment for running makefile and take screenshot</t>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>Set up github account, permission</t>
+  </si>
+  <si>
+    <t>Train team about existing code</t>
+  </si>
+  <si>
+    <t>Estimate budget</t>
+  </si>
+  <si>
+    <t>Get approval for budget</t>
+  </si>
+  <si>
+    <t>Create azure resources</t>
+  </si>
+  <si>
+    <t>Set up CI pipeline</t>
+  </si>
+  <si>
+    <t>Test CI pipeline</t>
+  </si>
+  <si>
+    <t>Set up CD pipeline</t>
+  </si>
+  <si>
+    <t>Test CD pipeline</t>
+  </si>
+  <si>
+    <t>Release and demo</t>
+  </si>
+  <si>
+    <t>Goals of year</t>
+  </si>
+  <si>
+    <t>Project manager guidelines</t>
+  </si>
+  <si>
+    <t>Deploy version successful</t>
+  </si>
+  <si>
+    <t>Demo every monday</t>
+  </si>
+  <si>
+    <t>Setup CI/CD</t>
+  </si>
+  <si>
+    <t>Enhance to deploy multi evironment</t>
+  </si>
+  <si>
+    <t>Report to team daily</t>
+  </si>
+  <si>
+    <t>Demo and document</t>
+  </si>
+  <si>
+    <t>Goals of quarter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Set up code</t>
+  </si>
+  <si>
+    <t>Update documents</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>1 : Easy</t>
+  </si>
+  <si>
+    <t>2 : Middle</t>
+  </si>
+  <si>
+    <t>3: Difficult</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,16 +132,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -127,14 +173,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,134 +492,205 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="85" customWidth="1"/>
+    <col min="3" max="3" width="44.77734375" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>44753</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>44753</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="C7">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="9"/>
+      <c r="B19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+      <c r="D20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+      <c r="C21" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+      <c r="D21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B26" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>15</v>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D22" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>